<commit_message>
alle libs inkludiert die notwendig sind, inserten von Kontakten geht, Selecten funktioniert serverseitig
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\JAVA-Projects\SWE2_GIT\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Datum</t>
   </si>
@@ -149,17 +144,20 @@
   </si>
   <si>
     <t>Alles etwas umgeschrieben, Daten werden korrekt an Proxy geschickt, DB etwas verändert (Adresse-Table)</t>
+  </si>
+  <si>
+    <t>Libs inkludiert, Programm lauffähig gemacht, Insert von Kontakten funktioniert, Selecten funktioniert serverseitig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -346,7 +344,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -423,7 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -435,13 +433,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -453,19 +451,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -474,37 +472,37 @@
     </xf>
   </cellXfs>
   <cellStyles count="62">
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Dezimal" xfId="15" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -535,7 +533,7 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
     <dxf>
@@ -838,9 +836,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -878,9 +876,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -912,10 +910,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -947,10 +944,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1123,14 +1119,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -1142,7 +1138,7 @@
     <col min="8" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1165,7 +1161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1">
       <c r="A2" s="6">
         <v>41754</v>
       </c>
@@ -1186,10 +1182,10 @@
       </c>
       <c r="G2" s="10">
         <f>(SUMIFS(D2:D1003,B2:B1003,F2) + SUMIFS(D2:D1003,B2:B1003,"Alle"))/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="6">
         <v>41761</v>
       </c>
@@ -1213,26 +1209,41 @@
         <v>6.833333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
+      <c r="A4" s="6">
+        <v>41763</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7">
+        <v>240</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="C5" s="26"/>
       <c r="F5" s="13"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1">
       <c r="C6" s="26"/>
       <c r="F6" s="15" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="16">
         <f>SUM(G2:G5)</f>
-        <v>6.833333333333333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+        <v>10.833333333333332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickTop="1"/>
+    <row r="69" spans="5:5">
       <c r="E69" s="25"/>
     </row>
   </sheetData>
@@ -1305,14 +1316,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1323,7 +1334,7 @@
     <col min="8" max="8" width="69.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -1349,7 +1360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1375,7 +1386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1401,7 +1412,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1427,7 +1438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1453,7 +1464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1479,7 +1490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1502,7 +1513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
         <v>28</v>
       </c>
@@ -1528,7 +1539,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1">
       <c r="D9" s="23">
         <f>SUM(D2:D8)</f>
         <v>36</v>
@@ -1538,37 +1549,37 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" thickTop="1">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1589,12 +1600,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Select funktioniert, Client/Proxy ausgebaut
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Datum</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Libs inkludiert, Programm lauffähig gemacht, Insert von Kontakten funktioniert, Selecten funktioniert serverseitig</t>
+  </si>
+  <si>
+    <t>Selecten funktionert komplett serverseitig, mit unterschiedlichen Eingaben</t>
+  </si>
+  <si>
+    <t>Selecten funktioniert im Zusammenspiel mit der GUI,  Proxy/Client verbessert</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1123,7 +1129,7 @@
   <dimension ref="A1:AMK69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1182,7 +1188,7 @@
       </c>
       <c r="G2" s="10">
         <f>(SUMIFS(D2:D1003,B2:B1003,F2) + SUMIFS(D2:D1003,B2:B1003,"Alle"))/60</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1228,18 +1234,46 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="C5" s="26"/>
+      <c r="A5" s="6">
+        <v>41764</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="7">
+        <v>120</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="C6" s="26"/>
+      <c r="A6" s="6">
+        <v>41765</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7">
+        <v>240</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="F6" s="15" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="16">
         <f>SUM(G2:G5)</f>
-        <v>10.833333333333332</v>
+        <v>16.833333333333332</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickTop="1"/>

</xml_diff>